<commit_message>
merge prototypes in one
Merge prototypes of ux test in one
Create unique script for the ux test
remove strange asset .xlsx
</commit_message>
<xml_diff>
--- a/UX-test/approve-reject/general-script-tasks.xlsx
+++ b/UX-test/approve-reject/general-script-tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylmejia/Documents/repos/repo-sketch-cactus/master/design-system/UX-test/approve-reject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CFA806-B72D-3548-9498-33E3B6B1C398}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C78B9C4-4ED4-C046-9A54-946F95ADD6C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="14600" xr2:uid="{69B89F32-9673-BB49-9CD2-9562BEC1F27F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Tasks</t>
   </si>
@@ -131,34 +131,37 @@
     <t>Name: General-flow-test - start on Dashboard page</t>
   </si>
   <si>
-    <t>Make a Commentary and use the "Pin" option</t>
-  </si>
-  <si>
-    <t>Make a commentary with a geometryc  figure (square or circle)</t>
-  </si>
-  <si>
-    <t>Select the live trace option on the                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          commentary and make it appear</t>
-  </si>
-  <si>
     <t>General comments</t>
   </si>
   <si>
-    <t>In scale 1-7, being 1 very dificult and 7 very easy how easy was to perform the "General-flow-test" tasks?</t>
-  </si>
-  <si>
-    <t>In scale 1-7, being 1 very dificult and 7 very easy how easy was to perform the "Asset-explorer-actions" tasks?</t>
-  </si>
-  <si>
     <t>Name: Image-viewer-actions - start on Image-details</t>
   </si>
   <si>
-    <t>In scale 1-7, being 1 very dificult and 7 very easy how easy was to perform the "Image-viewer-actions" tasks?</t>
-  </si>
-  <si>
     <t>If you have suggestions or comments regarding any page of the prototypes please write ir here</t>
   </si>
   <si>
     <t>Thank you for your time. The purpose of this test is to evaluate a new interface and general experience on the storage assets feature of the application Drive Plus. All your feedback is valuable and will help us determine if our UI-UX strategy is working as we expect. Please think aloud as much as possible to describe what you're looking at and what you're trying to do. This will be a big help. Be aware this is a prototype and not a final development so there are elements that can be not working or data that can be inconsistent because are not necessary for the current test. With your permission, we like to record the screen and the session, the recording will only be used to help us figure out how to improve the app, and it won't be seen by anyone except those with a need-to-know. Thank you so much again for your help.</t>
+  </si>
+  <si>
+    <t>Click on the image to add a comment</t>
+  </si>
+  <si>
+    <t>Select the geometic option comment</t>
+  </si>
+  <si>
+    <t>Select the live trace option on the                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          comment</t>
+  </si>
+  <si>
+    <t>Select the pin option, add some text and create a comment</t>
+  </si>
+  <si>
+    <t>In scale 1-7, being 1 very difficult and 7 very easy how easy was to perform the "General-flow-test" tasks?</t>
+  </si>
+  <si>
+    <t>In scale 1-7, being 1 very difficult and 7 very easy how easy was to perform the "Asset-explorer-actions" tasks?</t>
+  </si>
+  <si>
+    <t>In scale 1-7, being 1 very difficult and 7 very easy how easy was to perform the "Image-viewer-actions" tasks?</t>
   </si>
 </sst>
 </file>
@@ -777,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6657FE3D-C789-FA47-A22F-70453D6154E9}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,7 +799,7 @@
     </row>
     <row r="2" spans="1:3" ht="231" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -933,7 +936,7 @@
     </row>
     <row r="17" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -954,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C19" s="17"/>
     </row>
@@ -963,7 +966,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C20" s="18"/>
     </row>
@@ -972,41 +975,50 @@
         <v>3</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C21" s="19"/>
+    </row>
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="16">
+        <v>4</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="19"/>
     </row>
     <row r="23" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
     </row>
     <row r="24" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="23"/>
     </row>
     <row r="25" spans="1:3" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="23"/>
     </row>
     <row r="26" spans="1:3" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="24"/>
     </row>
     <row r="27" spans="1:3" ht="190" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="24"/>

</xml_diff>

<commit_message>
Changes on general test tasks
</commit_message>
<xml_diff>
--- a/UX-test/approve-reject/general-script-tasks.xlsx
+++ b/UX-test/approve-reject/general-script-tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylmejia/Documents/repos/repo-sketch-cactus/master/design-system/UX-test/approve-reject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C78B9C4-4ED4-C046-9A54-946F95ADD6C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F4B6792-37F8-F44A-A779-A30F3693E89E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="14600" xr2:uid="{69B89F32-9673-BB49-9CD2-9562BEC1F27F}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="14520" xr2:uid="{69B89F32-9673-BB49-9CD2-9562BEC1F27F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -422,45 +422,45 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -781,7 +781,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -791,11 +791,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
     </row>
     <row r="2" spans="1:3" ht="231" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
@@ -805,11 +805,11 @@
       <c r="C2" s="25"/>
     </row>
     <row r="3" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
     </row>
     <row r="4" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -823,10 +823,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12">
+      <c r="A5" s="24">
         <v>1</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -834,15 +834,15 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="11"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
@@ -870,11 +870,11 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="22"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -888,58 +888,58 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16">
+      <c r="A12" s="11">
         <v>1</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:3" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16">
+      <c r="A13" s="11">
         <v>2</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="13"/>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16">
+      <c r="A14" s="11">
         <v>3</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16">
+      <c r="A15" s="11">
         <v>4</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="C15" s="13"/>
     </row>
     <row r="16" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16">
+      <c r="A16" s="11">
         <v>5</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="18"/>
+      <c r="C16" s="13"/>
     </row>
     <row r="17" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
     </row>
     <row r="18" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -953,81 +953,86 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16">
+      <c r="A19" s="11">
         <v>1</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="17"/>
+      <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16">
+      <c r="A20" s="11">
         <v>2</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="18"/>
+      <c r="C20" s="13"/>
     </row>
     <row r="21" spans="1:3" ht="61" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="16">
+      <c r="A21" s="11">
         <v>3</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="19"/>
+      <c r="C21" s="14"/>
     </row>
     <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="16">
+      <c r="A22" s="11">
         <v>4</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="19"/>
+      <c r="C22" s="14"/>
     </row>
     <row r="23" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
     </row>
     <row r="24" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="23"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="17"/>
     </row>
     <row r="25" spans="1:3" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="23"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="17"/>
     </row>
     <row r="26" spans="1:3" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="24"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="18"/>
     </row>
     <row r="27" spans="1:3" ht="190" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="24"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="18"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B31" s="22"/>
+      <c r="B31" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A10:C10"/>
@@ -1035,11 +1040,6 @@
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes on prototype, Add new implementation of paginator on manual
</commit_message>
<xml_diff>
--- a/UX-test/approve-reject/general-script-tasks.xlsx
+++ b/UX-test/approve-reject/general-script-tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylmejia/Documents/repos/repo-sketch-cactus/master/design-system/UX-test/approve-reject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F4B6792-37F8-F44A-A779-A30F3693E89E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A341A8C-9099-8544-97E8-3AD8C46CE39E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="14520" xr2:uid="{69B89F32-9673-BB49-9CD2-9562BEC1F27F}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Tasks</t>
   </si>
   <si>
-    <t>Go to the assets of the project "Nintendo" and write the first comment of the following assets: Yoshi.jpg, Mario&amp;Princess.png and Bowser.jpg</t>
-  </si>
-  <si>
     <t>No.</t>
   </si>
   <si>
@@ -48,25 +45,49 @@
     <t xml:space="preserve">Comment Bowser.jpg: </t>
   </si>
   <si>
-    <t>Go to the asset Yoshi.jpg and write who was the last person that approve the version2 of the asset</t>
-  </si>
-  <si>
     <t>User name:</t>
   </si>
   <si>
-    <t>Go to Bowser.jpg approve the asset and told us the number of people that reject the asset</t>
-  </si>
-  <si>
     <t>Number of people who reject the asset:</t>
   </si>
   <si>
     <t>Introduction</t>
   </si>
   <si>
-    <t xml:space="preserve">Aprove o reject the asset that has been uploaded </t>
-  </si>
-  <si>
-    <t>Tell us how many assets are and describe for each one how many aproves, rejects and comments are</t>
+    <t>Name: Asset-explorer-actions - start on Asset-explorer page</t>
+  </si>
+  <si>
+    <t>Name: General-flow-test - start on Dashboard page</t>
+  </si>
+  <si>
+    <t>General comments</t>
+  </si>
+  <si>
+    <t>Name: Image-viewer-actions - start on Image-details</t>
+  </si>
+  <si>
+    <t>If you have suggestions or comments regarding any page of the prototypes please write ir here</t>
+  </si>
+  <si>
+    <t>Thank you for your time. The purpose of this test is to evaluate a new interface and general experience on the storage assets feature of the application Drive Plus. All your feedback is valuable and will help us determine if our UI-UX strategy is working as we expect. Please think aloud as much as possible to describe what you're looking at and what you're trying to do. This will be a big help. Be aware this is a prototype and not a final development so there are elements that can be not working or data that can be inconsistent because are not necessary for the current test. With your permission, we like to record the screen and the session, the recording will only be used to help us figure out how to improve the app, and it won't be seen by anyone except those with a need-to-know. Thank you so much again for your help.</t>
+  </si>
+  <si>
+    <t>Select the geometic option comment</t>
+  </si>
+  <si>
+    <t>Select the live trace option on the                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          comment</t>
+  </si>
+  <si>
+    <t>In scale 1-7, being 1 very difficult and 7 very easy how easy was to perform the "General-flow-test" tasks?</t>
+  </si>
+  <si>
+    <t>In scale 1-7, being 1 very difficult and 7 very easy how easy was to perform the "Asset-explorer-actions" tasks?</t>
+  </si>
+  <si>
+    <t>In scale 1-7, being 1 very difficult and 7 very easy how easy was to perform the "Image-viewer-actions" tasks?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No comment </t>
   </si>
   <si>
     <r>
@@ -78,7 +99,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Bowser.jpg</t>
+      <t>Number of assets:
+Bowser.jpg</t>
     </r>
     <r>
       <rPr>
@@ -116,52 +138,119 @@
     </r>
   </si>
   <si>
-    <t>Select each asset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select All assets and Aprove or Reject all </t>
-  </si>
-  <si>
-    <t>Upload the donkey.jpg image of images folder in the project nintendo.</t>
-  </si>
-  <si>
-    <t>Name: Asset-explorer-actions - start on Asset-explorer page</t>
-  </si>
-  <si>
-    <t>Name: General-flow-test - start on Dashboard page</t>
-  </si>
-  <si>
-    <t>General comments</t>
-  </si>
-  <si>
-    <t>Name: Image-viewer-actions - start on Image-details</t>
-  </si>
-  <si>
-    <t>If you have suggestions or comments regarding any page of the prototypes please write ir here</t>
-  </si>
-  <si>
-    <t>Thank you for your time. The purpose of this test is to evaluate a new interface and general experience on the storage assets feature of the application Drive Plus. All your feedback is valuable and will help us determine if our UI-UX strategy is working as we expect. Please think aloud as much as possible to describe what you're looking at and what you're trying to do. This will be a big help. Be aware this is a prototype and not a final development so there are elements that can be not working or data that can be inconsistent because are not necessary for the current test. With your permission, we like to record the screen and the session, the recording will only be used to help us figure out how to improve the app, and it won't be seen by anyone except those with a need-to-know. Thank you so much again for your help.</t>
-  </si>
-  <si>
-    <t>Click on the image to add a comment</t>
-  </si>
-  <si>
-    <t>Select the geometic option comment</t>
-  </si>
-  <si>
-    <t>Select the live trace option on the                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          comment</t>
-  </si>
-  <si>
-    <t>Select the pin option, add some text and create a comment</t>
-  </si>
-  <si>
-    <t>In scale 1-7, being 1 very difficult and 7 very easy how easy was to perform the "General-flow-test" tasks?</t>
-  </si>
-  <si>
-    <t>In scale 1-7, being 1 very difficult and 7 very easy how easy was to perform the "Asset-explorer-actions" tasks?</t>
-  </si>
-  <si>
-    <t>In scale 1-7, being 1 very difficult and 7 very easy how easy was to perform the "Image-viewer-actions" tasks?</t>
+    <t>Select one of the assets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on the image </t>
+  </si>
+  <si>
+    <t>add text and create a comment</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Approve</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reject</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the asset that has been uploaded </t>
+    </r>
+  </si>
+  <si>
+    <t>Go to Bowser.jpg approve the asset and write in the "notes" column the number of people that reject the asset</t>
+  </si>
+  <si>
+    <t>Go to the asset Yoshi.jpg and write on the "notes" column who was the last person that approve the version 2 of the asset</t>
+  </si>
+  <si>
+    <t>Go to the assets of the project "Nintendo" and write on the "notes" column the first comment of the following assets: Yoshi.jpg, Mario&amp;Princess.png and Bowser.jpg</t>
+  </si>
+  <si>
+    <t>Upload the donkey.jpg, the image that was on the email of this meeting</t>
+  </si>
+  <si>
+    <t>Write on the "notes" column how many assets are and describe for each one how many aproves, rejects and comments are</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Select all assets with one action and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Approve</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Reject</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> all </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -409,9 +498,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -426,9 +512,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -446,6 +529,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -455,14 +541,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -780,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6657FE3D-C789-FA47-A22F-70453D6154E9}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -791,248 +880,259 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22"/>
+      <c r="A1" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" ht="231" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
+      <c r="A2" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22"/>
+      <c r="A3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
     </row>
     <row r="4" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18">
+        <v>1</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="24">
-        <v>1</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4" t="s">
+    <row r="6" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="18"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="4" t="s">
+    <row r="7" spans="1:3" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>2</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>7</v>
+      <c r="B8" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>3</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="22"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
+        <v>1</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
+        <v>2</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11">
-        <v>1</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="12"/>
-    </row>
-    <row r="13" spans="1:3" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11">
-        <v>2</v>
-      </c>
-      <c r="B13" s="10" t="s">
+      <c r="B14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
+        <v>4</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>5</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="13"/>
-    </row>
-    <row r="14" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11">
-        <v>3</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11">
-        <v>4</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="13"/>
-    </row>
-    <row r="16" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
-        <v>5</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="13"/>
-    </row>
-    <row r="17" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="22"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
     </row>
     <row r="18" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>1</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10">
+        <v>2</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11">
-        <v>1</v>
-      </c>
-      <c r="B19" s="10" t="s">
+      <c r="B21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="10">
+        <v>4</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="12"/>
-    </row>
-    <row r="20" spans="1:3" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11">
-        <v>2</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="13"/>
-    </row>
-    <row r="21" spans="1:3" ht="61" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11">
-        <v>3</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="14"/>
-    </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="11">
-        <v>4</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="14"/>
+      <c r="C22" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="23" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
     </row>
     <row r="24" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="17"/>
+      <c r="A24" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="17"/>
+      <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:3" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="17"/>
+      <c r="A25" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="15"/>
     </row>
     <row r="26" spans="1:3" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="18"/>
+      <c r="A26" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="17"/>
+      <c r="C26" s="16"/>
     </row>
     <row r="27" spans="1:3" ht="190" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="18"/>
+      <c r="A27" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="16"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B31" s="16"/>
+      <c r="B31" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A10:C10"/>
@@ -1040,6 +1140,11 @@
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes on manual, excel script and prototypes
Changes on the .ts patterns adding alias on the imports
Changes on excel script
Last changes on prototype of Usability test to see arrow inmediatelly the user enter de documents viewer
</commit_message>
<xml_diff>
--- a/UX-test/approve-reject/general-script-tasks.xlsx
+++ b/UX-test/approve-reject/general-script-tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylmejia/Documents/repos/repo-sketch-cactus/master/design-system/UX-test/approve-reject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A341A8C-9099-8544-97E8-3AD8C46CE39E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645DD71E-7657-434E-B87F-2AF4D4C6690E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="14520" xr2:uid="{69B89F32-9673-BB49-9CD2-9562BEC1F27F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Tasks</t>
   </si>
@@ -138,25 +138,47 @@
     </r>
   </si>
   <si>
-    <t>Select one of the assets</t>
-  </si>
-  <si>
     <t xml:space="preserve">Click on the image </t>
   </si>
   <si>
-    <t>add text and create a comment</t>
-  </si>
-  <si>
+    <t>Write on the "notes" column how many assets are and describe for each one how many aproves, rejects and comments are</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Go to the asset Yoshi.jpg and write on the "notes" column who was the last person that </t>
+    </r>
     <r>
       <rPr>
         <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">approve </t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Approve</t>
+      <t>the version 2 of the asset</t>
+    </r>
+  </si>
+  <si>
+    <t>Go directly from the dashboard to the assets of the project "Nintendo". Enter to one of the three assets</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)_x0000_"/>
+      </rPr>
+      <t>Without going back</t>
     </r>
     <r>
       <rPr>
@@ -171,13 +193,30 @@
     <r>
       <rPr>
         <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)_x0000_"/>
+      </rPr>
+      <t>closing the viewer</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>reject</t>
+      <t xml:space="preserve"> go to the last screen, try to go to the different assets. Plase</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve"> copy and paste</t>
     </r>
     <r>
       <rPr>
@@ -187,38 +226,45 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> the asset that has been uploaded </t>
-    </r>
-  </si>
-  <si>
-    <t>Go to Bowser.jpg approve the asset and write in the "notes" column the number of people that reject the asset</t>
-  </si>
-  <si>
-    <t>Go to the asset Yoshi.jpg and write on the "notes" column who was the last person that approve the version 2 of the asset</t>
-  </si>
-  <si>
-    <t>Go to the assets of the project "Nintendo" and write on the "notes" column the first comment of the following assets: Yoshi.jpg, Mario&amp;Princess.png and Bowser.jpg</t>
-  </si>
-  <si>
-    <t>Upload the donkey.jpg, the image that was on the email of this meeting</t>
-  </si>
-  <si>
-    <t>Write on the "notes" column how many assets are and describe for each one how many aproves, rejects and comments are</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Select all assets with one action and </t>
+      <t xml:space="preserve"> in this excel on the column "notes" the last comment of the chat panel</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Go to Bowser.jpg</t>
     </r>
     <r>
       <rPr>
         <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve"> approve</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Approve</t>
+      <t xml:space="preserve"> the asset </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Write in the "notes" column the number of people that </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)_x0000_"/>
+      </rPr>
+      <t>approve</t>
     </r>
     <r>
       <rPr>
@@ -228,18 +274,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> or </t>
-    </r>
+      <t xml:space="preserve"> the asset</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)_x0000_"/>
+      </rPr>
+      <t>Approve</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Reject</t>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)_x0000_"/>
+      </rPr>
+      <t>reject</t>
     </r>
     <r>
       <rPr>
@@ -249,15 +314,85 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve"> the asset that has been uploaded </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)_x0000_"/>
+      </rPr>
+      <t>Upload the donkey.jpg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, the image that was on the email of this meeting</t>
+    </r>
+  </si>
+  <si>
+    <t>Check one of the assets</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Check all assets. With one action </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)_x0000_"/>
+      </rPr>
+      <t>Approve</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)_x0000_"/>
+      </rPr>
+      <t>Reject</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> all </t>
     </r>
+  </si>
+  <si>
+    <t>Add text and create a comment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -288,6 +423,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri (Cuerpo)_x0000_"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -315,7 +456,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -474,11 +615,120 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -489,18 +739,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -510,9 +754,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -526,32 +767,77 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -867,40 +1153,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6657FE3D-C789-FA47-A22F-70453D6154E9}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="50" customWidth="1"/>
     <col min="3" max="3" width="60" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:3" ht="40" customHeight="1">
+      <c r="A1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="21"/>
-    </row>
-    <row r="2" spans="1:3" ht="231" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
+    </row>
+    <row r="2" spans="1:3" ht="231" customHeight="1" thickBot="1">
+      <c r="A2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-    </row>
-    <row r="3" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+    </row>
+    <row r="3" spans="1:3" ht="35" customHeight="1">
+      <c r="A3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-    </row>
-    <row r="4" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+    </row>
+    <row r="4" spans="1:3" ht="53" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -911,240 +1197,263 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18">
+    <row r="5" spans="1:3" ht="31" customHeight="1">
+      <c r="A5" s="19">
         <v>1</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="32"/>
+    </row>
+    <row r="6" spans="1:3" ht="51" customHeight="1">
+      <c r="A6" s="19"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="32"/>
+    </row>
+    <row r="7" spans="1:3" ht="67" hidden="1" customHeight="1">
+      <c r="A7" s="19"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="32"/>
+    </row>
+    <row r="8" spans="1:3" ht="67" customHeight="1">
+      <c r="A8" s="29">
+        <v>2</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="67" customHeight="1">
+      <c r="A9" s="30"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="67" customHeight="1">
+      <c r="A10" s="31"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="56" customHeight="1">
+      <c r="A11" s="4">
+        <v>2</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="56" customHeight="1">
+      <c r="A12" s="21">
+        <v>3</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="36"/>
+    </row>
+    <row r="13" spans="1:3" ht="53" customHeight="1" thickBot="1">
+      <c r="A13" s="5">
+        <v>4</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C13" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="41" customHeight="1">
+      <c r="A14" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45" customHeight="1">
+      <c r="A16" s="8">
+        <v>1</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="33"/>
+    </row>
+    <row r="17" spans="1:3" ht="47" customHeight="1">
+      <c r="A17" s="8">
+        <v>2</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="34"/>
+    </row>
+    <row r="18" spans="1:3" ht="165" customHeight="1">
+      <c r="A18" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="4" t="s">
+      <c r="B18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="37" customHeight="1">
+      <c r="A19" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="4" t="s">
+      <c r="B19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="33"/>
+    </row>
+    <row r="20" spans="1:3" ht="35" customHeight="1" thickBot="1">
+      <c r="A20" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="B20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="33"/>
+    </row>
+    <row r="21" spans="1:3" ht="45" customHeight="1">
+      <c r="A21" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+    </row>
+    <row r="22" spans="1:3" ht="28" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+    </row>
+    <row r="23" spans="1:3" ht="35" customHeight="1">
+      <c r="A23" s="8">
+        <v>1</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="53" customHeight="1">
+      <c r="A24" s="8">
+        <v>2</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="61" customHeight="1">
+      <c r="A25" s="8">
         <v>3</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10">
-        <v>1</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="11" t="s">
+      <c r="B25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="33" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10">
-        <v>2</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="25" t="s">
+    <row r="26" spans="1:3" ht="17">
+      <c r="A26" s="8">
+        <v>4</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="33" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
-        <v>3</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10">
-        <v>4</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>5</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="21"/>
-    </row>
-    <row r="18" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
-        <v>1</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10">
-        <v>2</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="61" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10">
-        <v>3</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="10">
-        <v>4</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="23" t="s">
+    <row r="27" spans="1:3" ht="39" customHeight="1">
+      <c r="A27" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-    </row>
-    <row r="24" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+    </row>
+    <row r="28" spans="1:3" ht="51" customHeight="1">
+      <c r="A28" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="15"/>
-    </row>
-    <row r="25" spans="1:3" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
+      <c r="B28" s="24"/>
+      <c r="C28" s="12"/>
+    </row>
+    <row r="29" spans="1:3" ht="47" customHeight="1">
+      <c r="A29" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="15"/>
-    </row>
-    <row r="26" spans="1:3" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
+      <c r="B29" s="24"/>
+      <c r="C29" s="12"/>
+    </row>
+    <row r="30" spans="1:3" ht="55" customHeight="1">
+      <c r="A30" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="16"/>
-    </row>
-    <row r="27" spans="1:3" ht="190" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
+      <c r="B30" s="24"/>
+      <c r="C30" s="13"/>
+    </row>
+    <row r="31" spans="1:3" ht="190" customHeight="1">
+      <c r="A31" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="16"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B31" s="14"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="13"/>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
+  <mergeCells count="15">
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C5:C7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>